<commit_message>
update phieu muon + phieu nhap
</commit_message>
<xml_diff>
--- a/importPhieuNhap.xlsx
+++ b/importPhieuNhap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads_D\Thuvien\Thuvien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C86388-FE78-4E71-8697-4DA62AADF19D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC580368-A4F6-4607-B4E4-48F3777A1026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -440,7 +440,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>